<commit_message>
Add peak BDD size for XB worst case
</commit_message>
<xml_diff>
--- a/lockstep_algorithm/data/Full data.xlsx
+++ b/lockstep_algorithm/data/Full data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ablum\bachelorprojekt\lockstep_algorithm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D0014-3075-4E76-93B4-DD1C0B4C0C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170995F4-50A6-436E-97E2-92EFD8887CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{F15F8A2E-46BA-487E-9055-5E3E5DA9E31A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{F15F8A2E-46BA-487E-9055-5E3E5DA9E31A}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="58">
   <si>
     <t>Places</t>
   </si>
@@ -12163,7 +12163,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'XB slow'!$K$3:$K$8</c:f>
+              <c:f>'XB slow'!$M$3:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -12239,7 +12239,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'XB slow'!$L$3:$L$8</c:f>
+              <c:f>'XB slow'!$N$3:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -22148,7 +22148,7 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>509587</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -35560,37 +35560,41 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F5B0B3-5D4D-4178-B673-EB546C251537}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="94" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
       <c r="D1" s="96"/>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="94" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="95"/>
-      <c r="G1" s="94" t="s">
+      <c r="G1" s="96"/>
+      <c r="H1" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="96"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="95"/>
+      <c r="J1" s="96"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -35604,28 +35608,34 @@
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -35644,26 +35654,32 @@
       <c r="F3" s="2">
         <v>27273</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="32">
+        <v>113</v>
+      </c>
+      <c r="H3" s="1">
         <v>2504</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="2">
         <v>197670</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J8" si="0">MAX(F3,H3)</f>
+      <c r="J3" s="32">
+        <v>199</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="0">MAX(F3,I3)</f>
         <v>197670</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="1">F3/J3</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="1">F3/L3</f>
         <v>0.13797237820610109</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="2">H3/J3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="2">I3/L3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>200</v>
       </c>
@@ -35682,26 +35698,32 @@
       <c r="F4" s="2">
         <v>109817</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="32">
+        <v>218</v>
+      </c>
+      <c r="H4" s="1">
         <v>38785</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="2">
         <v>2310995</v>
       </c>
       <c r="J4" s="32">
+        <v>399</v>
+      </c>
+      <c r="L4" s="32">
         <f t="shared" si="0"/>
         <v>2310995</v>
       </c>
-      <c r="K4" s="32">
+      <c r="M4" s="32">
         <f t="shared" si="1"/>
         <v>4.7519358544696119E-2</v>
       </c>
-      <c r="L4" s="32">
+      <c r="N4" s="32">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>300</v>
       </c>
@@ -35720,26 +35742,32 @@
       <c r="F5" s="2">
         <v>248078</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="32">
+        <v>322</v>
+      </c>
+      <c r="H5" s="1">
         <v>133496</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="2">
         <v>7135070</v>
       </c>
       <c r="J5" s="32">
+        <v>599</v>
+      </c>
+      <c r="L5" s="32">
         <f t="shared" si="0"/>
         <v>7135070</v>
       </c>
-      <c r="K5" s="32">
+      <c r="M5" s="32">
         <f t="shared" si="1"/>
         <v>3.476882497298555E-2</v>
       </c>
-      <c r="L5" s="32">
+      <c r="N5" s="32">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>400</v>
       </c>
@@ -35758,26 +35786,32 @@
       <c r="F6" s="2">
         <v>442899</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="32">
+        <v>426</v>
+      </c>
+      <c r="H6" s="1">
         <v>315979</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="2">
         <v>15459995</v>
       </c>
       <c r="J6" s="32">
+        <v>799</v>
+      </c>
+      <c r="L6" s="32">
         <f t="shared" si="0"/>
         <v>15459995</v>
       </c>
-      <c r="K6" s="32">
+      <c r="M6" s="32">
         <f t="shared" si="1"/>
         <v>2.8648068773631557E-2</v>
       </c>
-      <c r="L6" s="32">
+      <c r="N6" s="32">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>500</v>
       </c>
@@ -35796,26 +35830,32 @@
       <c r="F7" s="2">
         <v>692464</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="32">
+        <v>529</v>
+      </c>
+      <c r="H7" s="1">
         <v>630470</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="2">
         <v>28075870</v>
       </c>
       <c r="J7" s="32">
+        <v>999</v>
+      </c>
+      <c r="L7" s="32">
         <f t="shared" si="0"/>
         <v>28075870</v>
       </c>
-      <c r="K7" s="32">
+      <c r="M7" s="32">
         <f t="shared" si="1"/>
         <v>2.4664026439786192E-2</v>
       </c>
-      <c r="L7" s="32">
+      <c r="N7" s="32">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>600</v>
       </c>
@@ -35834,30 +35874,36 @@
       <c r="F8" s="5">
         <v>999533</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="32">
+        <v>632</v>
+      </c>
+      <c r="H8" s="4">
         <v>1066631</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="5">
         <v>45772795</v>
       </c>
       <c r="J8" s="32">
+        <v>1199</v>
+      </c>
+      <c r="L8" s="32">
         <f t="shared" si="0"/>
         <v>45772795</v>
       </c>
-      <c r="K8" s="32">
+      <c r="M8" s="32">
         <f t="shared" si="1"/>
         <v>2.1836835613818207E-2</v>
       </c>
-      <c r="L8" s="32">
+      <c r="N8" s="32">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -37569,16 +37615,16 @@
     <sortCondition ref="C3:C20"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="K22:M22"/>
     <mergeCell ref="N22:P22"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -37589,7 +37635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1E843B-AFB3-4BF6-9378-10FF72A3078D}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -37645,15 +37691,15 @@
         <v>39</v>
       </c>
       <c r="F2" s="88">
-        <f>E2*2/B2/B2</f>
+        <f t="shared" ref="F2:F33" si="0">E2*2/B2/B2</f>
         <v>0.64462809917355368</v>
       </c>
       <c r="G2" s="82">
-        <f>E2/B2</f>
+        <f t="shared" ref="G2:G33" si="1">E2/B2</f>
         <v>3.5454545454545454</v>
       </c>
       <c r="H2" s="81">
-        <f>2*E2/(B2*(B2-1))</f>
+        <f t="shared" ref="H2:H33" si="2">2*E2/(B2*(B2-1))</f>
         <v>0.70909090909090911</v>
       </c>
       <c r="I2" s="87"/>
@@ -37675,15 +37721,15 @@
         <v>188</v>
       </c>
       <c r="F3" s="90">
-        <f>E3*2/B3/B3</f>
+        <f t="shared" si="0"/>
         <v>0.77685950413223137</v>
       </c>
       <c r="G3" s="85">
-        <f>E3/B3</f>
+        <f t="shared" si="1"/>
         <v>8.545454545454545</v>
       </c>
       <c r="H3" s="86">
-        <f>2*E3/(B3*(B3-1))</f>
+        <f t="shared" si="2"/>
         <v>0.81385281385281383</v>
       </c>
       <c r="I3" s="87"/>
@@ -37705,15 +37751,15 @@
         <v>80</v>
       </c>
       <c r="F4" s="88">
-        <f>E4*2/B4/B4</f>
+        <f t="shared" si="0"/>
         <v>0.44321329639889195</v>
       </c>
       <c r="G4" s="82">
-        <f>E4/B4</f>
+        <f t="shared" si="1"/>
         <v>4.2105263157894735</v>
       </c>
       <c r="H4" s="81">
-        <f>2*E4/(B4*(B4-1))</f>
+        <f t="shared" si="2"/>
         <v>0.46783625730994149</v>
       </c>
       <c r="I4" s="87"/>
@@ -37735,15 +37781,15 @@
         <v>98</v>
       </c>
       <c r="F5" s="88">
-        <f>E5*2/B5/B5</f>
+        <f t="shared" si="0"/>
         <v>0.67820069204152245</v>
       </c>
       <c r="G5" s="82">
-        <f>E5/B5</f>
+        <f t="shared" si="1"/>
         <v>5.7647058823529411</v>
       </c>
       <c r="H5" s="81">
-        <f>2*E5/(B5*(B5-1))</f>
+        <f t="shared" si="2"/>
         <v>0.72058823529411764</v>
       </c>
       <c r="I5" s="87"/>
@@ -37765,15 +37811,15 @@
         <v>218</v>
       </c>
       <c r="F6" s="90">
-        <f>E6*2/B6/B6</f>
+        <f t="shared" si="0"/>
         <v>0.51843043995243765</v>
       </c>
       <c r="G6" s="85">
-        <f>E6/B6</f>
+        <f t="shared" si="1"/>
         <v>7.5172413793103452</v>
       </c>
       <c r="H6" s="86">
-        <f>2*E6/(B6*(B6-1))</f>
+        <f t="shared" si="2"/>
         <v>0.53694581280788178</v>
       </c>
       <c r="I6" s="87"/>
@@ -37795,15 +37841,15 @@
         <v>121</v>
       </c>
       <c r="F7" s="88">
-        <f>E7*2/B7/B7</f>
+        <f t="shared" si="0"/>
         <v>0.3319615912208505</v>
       </c>
       <c r="G7" s="82">
-        <f>E7/B7</f>
+        <f t="shared" si="1"/>
         <v>4.4814814814814818</v>
       </c>
       <c r="H7" s="81">
-        <f>2*E7/(B7*(B7-1))</f>
+        <f t="shared" si="2"/>
         <v>0.34472934472934474</v>
       </c>
       <c r="I7" s="87"/>
@@ -37825,15 +37871,15 @@
         <v>148</v>
       </c>
       <c r="F8" s="88">
-        <f>E8*2/B8/B8</f>
+        <f t="shared" si="0"/>
         <v>0.67120181405895685</v>
       </c>
       <c r="G8" s="82">
-        <f>E8/B8</f>
+        <f t="shared" si="1"/>
         <v>7.0476190476190474</v>
       </c>
       <c r="H8" s="81">
-        <f>2*E8/(B8*(B8-1))</f>
+        <f t="shared" si="2"/>
         <v>0.70476190476190481</v>
       </c>
       <c r="I8" s="87"/>
@@ -37855,15 +37901,15 @@
         <v>481</v>
       </c>
       <c r="F9" s="90">
-        <f>E9*2/B9/B9</f>
+        <f t="shared" si="0"/>
         <v>0.5722784057108864</v>
       </c>
       <c r="G9" s="85">
-        <f>E9/B9</f>
+        <f t="shared" si="1"/>
         <v>11.731707317073171</v>
       </c>
       <c r="H9" s="86">
-        <f>2*E9/(B9*(B9-1))</f>
+        <f t="shared" si="2"/>
         <v>0.5865853658536585</v>
       </c>
       <c r="I9" s="87"/>
@@ -37885,15 +37931,15 @@
         <v>298</v>
       </c>
       <c r="F10" s="90">
-        <f>E10*2/B10/B10</f>
+        <f t="shared" si="0"/>
         <v>0.70868014268727708</v>
       </c>
       <c r="G10" s="85">
-        <f>E10/B10</f>
+        <f t="shared" si="1"/>
         <v>10.275862068965518</v>
       </c>
       <c r="H10" s="86">
-        <f>2*E10/(B10*(B10-1))</f>
+        <f t="shared" si="2"/>
         <v>0.73399014778325122</v>
       </c>
       <c r="I10" s="87"/>
@@ -37915,15 +37961,15 @@
         <v>162</v>
       </c>
       <c r="F11" s="88">
-        <f>E11*2/B11/B11</f>
+        <f t="shared" si="0"/>
         <v>0.26448979591836735</v>
       </c>
       <c r="G11" s="82">
-        <f>E11/B11</f>
+        <f t="shared" si="1"/>
         <v>4.628571428571429</v>
       </c>
       <c r="H11" s="81">
-        <f>2*E11/(B11*(B11-1))</f>
+        <f t="shared" si="2"/>
         <v>0.27226890756302519</v>
       </c>
       <c r="I11" s="87"/>
@@ -37945,15 +37991,15 @@
         <v>2372</v>
       </c>
       <c r="F12" s="90">
-        <f>E12*2/B12/B12</f>
+        <f t="shared" si="0"/>
         <v>0.3715247865925288</v>
       </c>
       <c r="G12" s="85">
-        <f>E12/B12</f>
+        <f t="shared" si="1"/>
         <v>20.991150442477878</v>
       </c>
       <c r="H12" s="86">
-        <f>2*E12/(B12*(B12-1))</f>
+        <f t="shared" si="2"/>
         <v>0.37484197218710491</v>
       </c>
       <c r="I12" s="87"/>
@@ -37975,15 +38021,15 @@
         <v>574</v>
       </c>
       <c r="F13" s="90">
-        <f>E13*2/B13/B13</f>
+        <f t="shared" si="0"/>
         <v>0.478134110787172</v>
       </c>
       <c r="G13" s="85">
-        <f>E13/B13</f>
+        <f t="shared" si="1"/>
         <v>11.714285714285714</v>
       </c>
       <c r="H13" s="86">
-        <f>2*E13/(B13*(B13-1))</f>
+        <f t="shared" si="2"/>
         <v>0.48809523809523808</v>
       </c>
       <c r="I13" s="87"/>
@@ -38005,15 +38051,15 @@
         <v>2865</v>
       </c>
       <c r="F14" s="90">
-        <f>E14*2/B14/B14</f>
+        <f t="shared" si="0"/>
         <v>0.35526071052142105</v>
       </c>
       <c r="G14" s="85">
-        <f>E14/B14</f>
+        <f t="shared" si="1"/>
         <v>22.559055118110237</v>
       </c>
       <c r="H14" s="86">
-        <f>2*E14/(B14*(B14-1))</f>
+        <f t="shared" si="2"/>
         <v>0.35808023997000377</v>
       </c>
       <c r="I14" s="87"/>
@@ -38035,15 +38081,15 @@
         <v>201</v>
       </c>
       <c r="F15" s="88">
-        <f>E15*2/B15/B15</f>
+        <f t="shared" si="0"/>
         <v>0.41831425598335065</v>
       </c>
       <c r="G15" s="82">
-        <f>E15/B15</f>
+        <f t="shared" si="1"/>
         <v>6.4838709677419351</v>
       </c>
       <c r="H15" s="81">
-        <f>2*E15/(B15*(B15-1))</f>
+        <f t="shared" si="2"/>
         <v>0.43225806451612903</v>
       </c>
       <c r="I15" s="87"/>
@@ -38065,15 +38111,15 @@
         <v>508</v>
       </c>
       <c r="F16" s="90">
-        <f>E16*2/B16/B16</f>
+        <f t="shared" si="0"/>
         <v>0.44097222222222227</v>
       </c>
       <c r="G16" s="85">
-        <f>E16/B16</f>
+        <f t="shared" si="1"/>
         <v>10.583333333333334</v>
       </c>
       <c r="H16" s="86">
-        <f>2*E16/(B16*(B16-1))</f>
+        <f t="shared" si="2"/>
         <v>0.450354609929078</v>
       </c>
       <c r="I16" s="87"/>
@@ -38095,15 +38141,15 @@
         <v>203</v>
       </c>
       <c r="F17" s="88">
-        <f>E17*2/B17/B17</f>
+        <f t="shared" si="0"/>
         <v>0.21957815035154138</v>
       </c>
       <c r="G17" s="82">
-        <f>E17/B17</f>
+        <f t="shared" si="1"/>
         <v>4.7209302325581399</v>
       </c>
       <c r="H17" s="81">
-        <f>2*E17/(B17*(B17-1))</f>
+        <f t="shared" si="2"/>
         <v>0.22480620155038761</v>
       </c>
       <c r="I17" s="87"/>
@@ -38125,15 +38171,15 @@
         <v>3528</v>
       </c>
       <c r="F18" s="90">
-        <f>E18*2/B18/B18</f>
+        <f t="shared" si="0"/>
         <v>0.33560047562425682</v>
       </c>
       <c r="G18" s="85">
-        <f>E18/B18</f>
+        <f t="shared" si="1"/>
         <v>24.331034482758621</v>
       </c>
       <c r="H18" s="86">
-        <f>2*E18/(B18*(B18-1))</f>
+        <f t="shared" si="2"/>
         <v>0.33793103448275863</v>
       </c>
       <c r="I18" s="87"/>
@@ -38155,15 +38201,15 @@
         <v>783</v>
       </c>
       <c r="F19" s="90">
-        <f>E19*2/B19/B19</f>
+        <f t="shared" si="0"/>
         <v>0.435</v>
       </c>
       <c r="G19" s="85">
-        <f>E19/B19</f>
+        <f t="shared" si="1"/>
         <v>13.05</v>
       </c>
       <c r="H19" s="86">
-        <f>2*E19/(B19*(B19-1))</f>
+        <f t="shared" si="2"/>
         <v>0.44237288135593222</v>
       </c>
       <c r="I19" s="87"/>
@@ -38185,15 +38231,15 @@
         <v>380</v>
       </c>
       <c r="F20" s="90">
-        <f>E20*2/B20/B20</f>
+        <f t="shared" si="0"/>
         <v>0.27055891776432894</v>
       </c>
       <c r="G20" s="85">
-        <f>E20/B20</f>
+        <f t="shared" si="1"/>
         <v>7.1698113207547172</v>
       </c>
       <c r="H20" s="86">
-        <f>2*E20/(B20*(B20-1))</f>
+        <f t="shared" si="2"/>
         <v>0.27576197387518142</v>
       </c>
       <c r="I20" s="87"/>
@@ -38215,15 +38261,15 @@
         <v>301</v>
       </c>
       <c r="F21" s="88">
-        <f>E21*2/B21/B21</f>
+        <f t="shared" si="0"/>
         <v>0.39579224194608809</v>
       </c>
       <c r="G21" s="82">
-        <f>E21/B21</f>
+        <f t="shared" si="1"/>
         <v>7.7179487179487181</v>
       </c>
       <c r="H21" s="81">
-        <f>2*E21/(B21*(B21-1))</f>
+        <f t="shared" si="2"/>
         <v>0.40620782726045884</v>
       </c>
       <c r="I21" s="87"/>
@@ -38245,15 +38291,15 @@
         <v>304</v>
       </c>
       <c r="F22" s="88">
-        <f>E22*2/B22/B22</f>
+        <f t="shared" si="0"/>
         <v>0.30024691358024691</v>
       </c>
       <c r="G22" s="82">
-        <f>E22/B22</f>
+        <f t="shared" si="1"/>
         <v>6.7555555555555555</v>
       </c>
       <c r="H22" s="81">
-        <f>2*E22/(B22*(B22-1))</f>
+        <f t="shared" si="2"/>
         <v>0.30707070707070705</v>
       </c>
       <c r="I22" s="87"/>
@@ -38275,15 +38321,15 @@
         <v>823</v>
       </c>
       <c r="F23" s="90">
-        <f>E23*2/B23/B23</f>
+        <f t="shared" si="0"/>
         <v>0.37786960514233237</v>
       </c>
       <c r="G23" s="85">
-        <f>E23/B23</f>
+        <f t="shared" si="1"/>
         <v>12.469696969696969</v>
       </c>
       <c r="H23" s="86">
-        <f>2*E23/(B23*(B23-1))</f>
+        <f t="shared" si="2"/>
         <v>0.3836829836829837</v>
       </c>
       <c r="I23" s="87"/>
@@ -38305,15 +38351,15 @@
         <v>650</v>
       </c>
       <c r="F24" s="90">
-        <f>E24*2/B24/B24</f>
+        <f t="shared" si="0"/>
         <v>0.2811418685121107</v>
       </c>
       <c r="G24" s="85">
-        <f>E24/B24</f>
+        <f t="shared" si="1"/>
         <v>9.5588235294117645</v>
       </c>
       <c r="H24" s="86">
-        <f>2*E24/(B24*(B24-1))</f>
+        <f t="shared" si="2"/>
         <v>0.28533801580333629</v>
       </c>
       <c r="I24" s="87"/>
@@ -38335,15 +38381,15 @@
         <v>454</v>
       </c>
       <c r="F25" s="88">
-        <f>E25*2/B25/B25</f>
+        <f t="shared" si="0"/>
         <v>0.27947060634041243</v>
       </c>
       <c r="G25" s="82">
-        <f>E25/B25</f>
+        <f t="shared" si="1"/>
         <v>7.9649122807017543</v>
       </c>
       <c r="H25" s="81">
-        <f>2*E25/(B25*(B25-1))</f>
+        <f t="shared" si="2"/>
         <v>0.28446115288220553</v>
       </c>
       <c r="I25" s="87"/>
@@ -38365,15 +38411,15 @@
         <v>407</v>
       </c>
       <c r="F26" s="88">
-        <f>E26*2/B26/B26</f>
+        <f t="shared" si="0"/>
         <v>0.23384085033036484</v>
       </c>
       <c r="G26" s="82">
-        <f>E26/B26</f>
+        <f t="shared" si="1"/>
         <v>6.898305084745763</v>
       </c>
       <c r="H26" s="81">
-        <f>2*E26/(B26*(B26-1))</f>
+        <f t="shared" si="2"/>
         <v>0.23787258912916423</v>
       </c>
       <c r="I26" s="87"/>
@@ -38395,15 +38441,15 @@
         <v>408</v>
       </c>
       <c r="F27" s="88">
-        <f>E27*2/B27/B27</f>
+        <f t="shared" si="0"/>
         <v>0.11844970242415445</v>
       </c>
       <c r="G27" s="82">
-        <f>E27/B27</f>
+        <f t="shared" si="1"/>
         <v>4.9156626506024095</v>
       </c>
       <c r="H27" s="81">
-        <f>2*E27/(B27*(B27-1))</f>
+        <f t="shared" si="2"/>
         <v>0.11989421099030267</v>
       </c>
       <c r="I27" s="87"/>
@@ -38425,15 +38471,15 @@
         <v>510</v>
       </c>
       <c r="F28" s="88">
-        <f>E28*2/B28/B28</f>
+        <f t="shared" si="0"/>
         <v>0.19140551698254832</v>
       </c>
       <c r="G28" s="82">
-        <f>E28/B28</f>
+        <f t="shared" si="1"/>
         <v>6.9863013698630141</v>
       </c>
       <c r="H28" s="81">
-        <f>2*E28/(B28*(B28-1))</f>
+        <f t="shared" si="2"/>
         <v>0.19406392694063926</v>
       </c>
       <c r="I28" s="87"/>
@@ -38455,15 +38501,15 @@
         <v>607</v>
       </c>
       <c r="F29" s="88">
-        <f>E29*2/B29/B29</f>
+        <f t="shared" si="0"/>
         <v>0.21582222222222222</v>
       </c>
       <c r="G29" s="82">
-        <f>E29/B29</f>
+        <f t="shared" si="1"/>
         <v>8.0933333333333337</v>
       </c>
       <c r="H29" s="81">
-        <f>2*E29/(B29*(B29-1))</f>
+        <f t="shared" si="2"/>
         <v>0.21873873873873872</v>
       </c>
       <c r="I29" s="87"/>
@@ -38485,15 +38531,15 @@
         <v>760</v>
       </c>
       <c r="F30" s="88">
-        <f>E30*2/B30/B30</f>
+        <f t="shared" si="0"/>
         <v>0.17574286044629436</v>
       </c>
       <c r="G30" s="82">
-        <f>E30/B30</f>
+        <f t="shared" si="1"/>
         <v>8.172043010752688</v>
       </c>
       <c r="H30" s="81">
-        <f>2*E30/(B30*(B30-1))</f>
+        <f t="shared" si="2"/>
         <v>0.17765310892940628</v>
       </c>
       <c r="I30" s="87"/>
@@ -38515,15 +38561,15 @@
         <v>2750</v>
       </c>
       <c r="F31" s="90">
-        <f>E31*2/B31/B31</f>
+        <f t="shared" si="0"/>
         <v>0.21755468533681421</v>
       </c>
       <c r="G31" s="85">
-        <f>E31/B31</f>
+        <f t="shared" si="1"/>
         <v>17.29559748427673</v>
       </c>
       <c r="H31" s="86">
-        <f>2*E31/(B31*(B31-1))</f>
+        <f t="shared" si="2"/>
         <v>0.2189316137250219</v>
       </c>
       <c r="I31" s="87"/>
@@ -38545,15 +38591,15 @@
         <v>818</v>
       </c>
       <c r="F32" s="88">
-        <f>E32*2/B32/B32</f>
+        <f t="shared" si="0"/>
         <v>6.1575520343257181E-2</v>
       </c>
       <c r="G32" s="82">
-        <f>E32/B32</f>
+        <f t="shared" si="1"/>
         <v>5.0184049079754605</v>
       </c>
       <c r="H32" s="81">
-        <f>2*E32/(B32*(B32-1))</f>
+        <f t="shared" si="2"/>
         <v>6.1955616147845186E-2</v>
       </c>
       <c r="I32" s="87"/>
@@ -38575,15 +38621,15 @@
         <v>1025</v>
       </c>
       <c r="F33" s="89">
-        <f>E33*2/B33/B33</f>
+        <f t="shared" si="0"/>
         <v>0.10024940094870165</v>
       </c>
       <c r="G33" s="83">
-        <f>E33/B33</f>
+        <f t="shared" si="1"/>
         <v>7.1678321678321675</v>
       </c>
       <c r="H33" s="84">
-        <f>2*E33/(B33*(B33-1))</f>
+        <f t="shared" si="2"/>
         <v>0.10095538264552349</v>
       </c>
       <c r="I33" s="87"/>
@@ -38632,15 +38678,15 @@
         <v>39</v>
       </c>
       <c r="F36" s="88">
-        <f t="shared" ref="F36:F67" si="0">E36*2/B36/B36</f>
+        <f t="shared" ref="F36:F67" si="3">E36*2/B36/B36</f>
         <v>0.64462809917355368</v>
       </c>
       <c r="G36" s="82">
-        <f t="shared" ref="G36:G67" si="1">E36/B36</f>
+        <f t="shared" ref="G36:G67" si="4">E36/B36</f>
         <v>3.5454545454545454</v>
       </c>
       <c r="H36" s="81">
-        <f t="shared" ref="H36:H67" si="2">2*E36/(B36*(B36-1))</f>
+        <f t="shared" ref="H36:H67" si="5">2*E36/(B36*(B36-1))</f>
         <v>0.70909090909090911</v>
       </c>
     </row>
@@ -38661,15 +38707,15 @@
         <v>80</v>
       </c>
       <c r="F37" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.44321329639889195</v>
       </c>
       <c r="G37" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.2105263157894735</v>
       </c>
       <c r="H37" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.46783625730994149</v>
       </c>
     </row>
@@ -38690,15 +38736,15 @@
         <v>121</v>
       </c>
       <c r="F38" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.3319615912208505</v>
       </c>
       <c r="G38" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.4814814814814818</v>
       </c>
       <c r="H38" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.34472934472934474</v>
       </c>
     </row>
@@ -38719,15 +38765,15 @@
         <v>162</v>
       </c>
       <c r="F39" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.26448979591836735</v>
       </c>
       <c r="G39" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.628571428571429</v>
       </c>
       <c r="H39" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.27226890756302519</v>
       </c>
     </row>
@@ -38748,15 +38794,15 @@
         <v>203</v>
       </c>
       <c r="F40" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.21957815035154138</v>
       </c>
       <c r="G40" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.7209302325581399</v>
       </c>
       <c r="H40" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.22480620155038761</v>
       </c>
     </row>
@@ -38777,15 +38823,15 @@
         <v>408</v>
       </c>
       <c r="F41" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.11844970242415445</v>
       </c>
       <c r="G41" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.9156626506024095</v>
       </c>
       <c r="H41" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.11989421099030267</v>
       </c>
     </row>
@@ -38806,15 +38852,15 @@
         <v>818</v>
       </c>
       <c r="F42" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.1575520343257181E-2</v>
       </c>
       <c r="G42" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.0184049079754605</v>
       </c>
       <c r="H42" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.1955616147845186E-2</v>
       </c>
     </row>
@@ -38835,15 +38881,15 @@
         <v>98</v>
       </c>
       <c r="F43" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.67820069204152245</v>
       </c>
       <c r="G43" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.7647058823529411</v>
       </c>
       <c r="H43" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.72058823529411764</v>
       </c>
     </row>
@@ -38864,15 +38910,15 @@
         <v>201</v>
       </c>
       <c r="F44" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.41831425598335065</v>
       </c>
       <c r="G44" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.4838709677419351</v>
       </c>
       <c r="H44" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.43225806451612903</v>
       </c>
     </row>
@@ -38893,15 +38939,15 @@
         <v>304</v>
       </c>
       <c r="F45" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.30024691358024691</v>
       </c>
       <c r="G45" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.7555555555555555</v>
       </c>
       <c r="H45" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.30707070707070705</v>
       </c>
     </row>
@@ -38922,15 +38968,15 @@
         <v>407</v>
       </c>
       <c r="F46" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.23384085033036484</v>
       </c>
       <c r="G46" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.898305084745763</v>
       </c>
       <c r="H46" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.23787258912916423</v>
       </c>
     </row>
@@ -38951,15 +38997,15 @@
         <v>510</v>
       </c>
       <c r="F47" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.19140551698254832</v>
       </c>
       <c r="G47" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.9863013698630141</v>
       </c>
       <c r="H47" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.19406392694063926</v>
       </c>
     </row>
@@ -38980,15 +39026,15 @@
         <v>148</v>
       </c>
       <c r="F48" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.67120181405895685</v>
       </c>
       <c r="G48" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7.0476190476190474</v>
       </c>
       <c r="H48" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.70476190476190481</v>
       </c>
     </row>
@@ -39009,15 +39055,15 @@
         <v>1025</v>
       </c>
       <c r="F49" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.10024940094870165</v>
       </c>
       <c r="G49" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7.1678321678321675</v>
       </c>
       <c r="H49" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.10095538264552349</v>
       </c>
     </row>
@@ -39038,15 +39084,15 @@
         <v>380</v>
       </c>
       <c r="F50" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27055891776432894</v>
       </c>
       <c r="G50" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7.1698113207547172</v>
       </c>
       <c r="H50" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.27576197387518142</v>
       </c>
     </row>
@@ -39067,15 +39113,15 @@
         <v>218</v>
       </c>
       <c r="F51" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.51843043995243765</v>
       </c>
       <c r="G51" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7.5172413793103452</v>
       </c>
       <c r="H51" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.53694581280788178</v>
       </c>
     </row>
@@ -39096,15 +39142,15 @@
         <v>301</v>
       </c>
       <c r="F52" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.39579224194608809</v>
       </c>
       <c r="G52" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7.7179487179487181</v>
       </c>
       <c r="H52" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.40620782726045884</v>
       </c>
     </row>
@@ -39125,15 +39171,15 @@
         <v>454</v>
       </c>
       <c r="F53" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27947060634041243</v>
       </c>
       <c r="G53" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7.9649122807017543</v>
       </c>
       <c r="H53" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.28446115288220553</v>
       </c>
     </row>
@@ -39154,15 +39200,15 @@
         <v>607</v>
       </c>
       <c r="F54" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.21582222222222222</v>
       </c>
       <c r="G54" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.0933333333333337</v>
       </c>
       <c r="H54" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.21873873873873872</v>
       </c>
     </row>
@@ -39183,15 +39229,15 @@
         <v>760</v>
       </c>
       <c r="F55" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.17574286044629436</v>
       </c>
       <c r="G55" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.172043010752688</v>
       </c>
       <c r="H55" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.17765310892940628</v>
       </c>
     </row>
@@ -39212,15 +39258,15 @@
         <v>188</v>
       </c>
       <c r="F56" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.77685950413223137</v>
       </c>
       <c r="G56" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.545454545454545</v>
       </c>
       <c r="H56" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.81385281385281383</v>
       </c>
     </row>
@@ -39241,15 +39287,15 @@
         <v>650</v>
       </c>
       <c r="F57" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.2811418685121107</v>
       </c>
       <c r="G57" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.5588235294117645</v>
       </c>
       <c r="H57" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.28533801580333629</v>
       </c>
     </row>
@@ -39270,15 +39316,15 @@
         <v>298</v>
       </c>
       <c r="F58" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.70868014268727708</v>
       </c>
       <c r="G58" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.275862068965518</v>
       </c>
       <c r="H58" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.73399014778325122</v>
       </c>
     </row>
@@ -39299,15 +39345,15 @@
         <v>508</v>
       </c>
       <c r="F59" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.44097222222222227</v>
       </c>
       <c r="G59" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.583333333333334</v>
       </c>
       <c r="H59" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.450354609929078</v>
       </c>
     </row>
@@ -39328,15 +39374,15 @@
         <v>574</v>
       </c>
       <c r="F60" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.478134110787172</v>
       </c>
       <c r="G60" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11.714285714285714</v>
       </c>
       <c r="H60" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.48809523809523808</v>
       </c>
     </row>
@@ -39357,15 +39403,15 @@
         <v>481</v>
       </c>
       <c r="F61" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5722784057108864</v>
       </c>
       <c r="G61" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11.731707317073171</v>
       </c>
       <c r="H61" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5865853658536585</v>
       </c>
     </row>
@@ -39386,15 +39432,15 @@
         <v>823</v>
       </c>
       <c r="F62" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.37786960514233237</v>
       </c>
       <c r="G62" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12.469696969696969</v>
       </c>
       <c r="H62" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.3836829836829837</v>
       </c>
     </row>
@@ -39415,15 +39461,15 @@
         <v>783</v>
       </c>
       <c r="F63" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.435</v>
       </c>
       <c r="G63" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13.05</v>
       </c>
       <c r="H63" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.44237288135593222</v>
       </c>
     </row>
@@ -39444,15 +39490,15 @@
         <v>2750</v>
       </c>
       <c r="F64" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.21755468533681421</v>
       </c>
       <c r="G64" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17.29559748427673</v>
       </c>
       <c r="H64" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.2189316137250219</v>
       </c>
     </row>
@@ -39473,15 +39519,15 @@
         <v>2372</v>
       </c>
       <c r="F65" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.3715247865925288</v>
       </c>
       <c r="G65" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20.991150442477878</v>
       </c>
       <c r="H65" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.37484197218710491</v>
       </c>
     </row>
@@ -39502,15 +39548,15 @@
         <v>2865</v>
       </c>
       <c r="F66" s="90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.35526071052142105</v>
       </c>
       <c r="G66" s="85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>22.559055118110237</v>
       </c>
       <c r="H66" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.35808023997000377</v>
       </c>
     </row>
@@ -39531,15 +39577,15 @@
         <v>3528</v>
       </c>
       <c r="F67" s="91">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.33560047562425682</v>
       </c>
       <c r="G67" s="92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>24.331034482758621</v>
       </c>
       <c r="H67" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.33793103448275863</v>
       </c>
     </row>

</xml_diff>